<commit_message>
Added design and updated hours.
</commit_message>
<xml_diff>
--- a/stundenlisten/Stundenliste-AlexanderSchmid.xlsx
+++ b/stundenlisten/Stundenliste-AlexanderSchmid.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexa\PRJ\HSP-RPOSC-Redpitaya-Oszilloskop\stundenlisten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A659B70-9F56-4AE2-9696-511384B78FBC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BA3A165-6015-466D-AE9D-02CB2AE9C452}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BE701AB6-5A3E-442C-8219-9B93BD6F3CD4}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Datum</t>
   </si>
@@ -73,6 +73,12 @@
   </si>
   <si>
     <t>Absprache mit Sebastian Ederer bezüglich Systemarchitektur und UI-Mockup</t>
+  </si>
+  <si>
+    <t>Implementierung bidirektionale Kommunikation zwischen Client und Server, Evaluation von libsigrok</t>
+  </si>
+  <si>
+    <t>Diskussion UI-Mockup</t>
   </si>
 </sst>
 </file>
@@ -461,7 +467,7 @@
   <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -605,153 +611,171 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>44154</v>
+      </c>
+      <c r="B11">
+        <v>4</v>
+      </c>
       <c r="C11">
         <f t="shared" si="0"/>
-        <v>14.5</v>
+        <v>18.5</v>
+      </c>
+      <c r="D11" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>44156</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
       <c r="C12">
         <f t="shared" si="0"/>
-        <v>14.5</v>
+        <v>19.5</v>
+      </c>
+      <c r="D12" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C13">
         <f t="shared" si="0"/>
-        <v>14.5</v>
+        <v>19.5</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C14">
         <f t="shared" si="0"/>
-        <v>14.5</v>
+        <v>19.5</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C15">
         <f t="shared" si="0"/>
-        <v>14.5</v>
+        <v>19.5</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C16">
         <f t="shared" si="0"/>
-        <v>14.5</v>
+        <v>19.5</v>
       </c>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C17">
         <f t="shared" si="0"/>
-        <v>14.5</v>
+        <v>19.5</v>
       </c>
     </row>
     <row r="18" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C18">
         <f t="shared" si="0"/>
-        <v>14.5</v>
+        <v>19.5</v>
       </c>
     </row>
     <row r="19" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C19">
         <f t="shared" si="0"/>
-        <v>14.5</v>
+        <v>19.5</v>
       </c>
     </row>
     <row r="20" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C20">
         <f t="shared" si="0"/>
-        <v>14.5</v>
+        <v>19.5</v>
       </c>
     </row>
     <row r="21" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C21">
         <f t="shared" si="0"/>
-        <v>14.5</v>
+        <v>19.5</v>
       </c>
     </row>
     <row r="22" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C22">
         <f t="shared" si="0"/>
-        <v>14.5</v>
+        <v>19.5</v>
       </c>
     </row>
     <row r="23" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C23">
         <f t="shared" si="0"/>
-        <v>14.5</v>
+        <v>19.5</v>
       </c>
     </row>
     <row r="24" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C24">
         <f t="shared" si="0"/>
-        <v>14.5</v>
+        <v>19.5</v>
       </c>
     </row>
     <row r="25" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C25">
         <f t="shared" si="0"/>
-        <v>14.5</v>
+        <v>19.5</v>
       </c>
     </row>
     <row r="26" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C26">
         <f t="shared" si="0"/>
-        <v>14.5</v>
+        <v>19.5</v>
       </c>
     </row>
     <row r="27" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C27">
         <f t="shared" si="0"/>
-        <v>14.5</v>
+        <v>19.5</v>
       </c>
     </row>
     <row r="28" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C28">
         <f t="shared" si="0"/>
-        <v>14.5</v>
+        <v>19.5</v>
       </c>
     </row>
     <row r="29" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C29">
         <f t="shared" si="0"/>
-        <v>14.5</v>
+        <v>19.5</v>
       </c>
     </row>
     <row r="30" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C30">
         <f t="shared" si="0"/>
-        <v>14.5</v>
+        <v>19.5</v>
       </c>
     </row>
     <row r="31" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C31">
         <f t="shared" si="0"/>
-        <v>14.5</v>
+        <v>19.5</v>
       </c>
     </row>
     <row r="32" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C32">
         <f t="shared" si="0"/>
-        <v>14.5</v>
+        <v>19.5</v>
       </c>
     </row>
     <row r="33" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C33">
         <f t="shared" si="0"/>
-        <v>14.5</v>
+        <v>19.5</v>
       </c>
     </row>
     <row r="34" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C34">
         <f t="shared" si="0"/>
-        <v>14.5</v>
+        <v>19.5</v>
       </c>
     </row>
     <row r="35" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C35">
         <f t="shared" si="0"/>
-        <v>14.5</v>
+        <v>19.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added design and hours
</commit_message>
<xml_diff>
--- a/stundenlisten/Stundenliste-AlexanderSchmid.xlsx
+++ b/stundenlisten/Stundenliste-AlexanderSchmid.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexa\PRJ\HSP-RPOSC-Redpitaya-Oszilloskop\stundenlisten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4041523-A21B-4221-81F5-B8756A79A1B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04B615B7-2A55-4599-B3C3-2F5E1486F1D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BE701AB6-5A3E-442C-8219-9B93BD6F3CD4}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
   <si>
     <t>Datum</t>
   </si>
@@ -100,6 +100,12 @@
   </si>
   <si>
     <t>Akquirierung der Testdaten für UART-Test, forum-post geschrieben</t>
+  </si>
+  <si>
+    <t>Wöchentliches Meeting + Vorbereitung</t>
+  </si>
+  <si>
+    <t>Einrichtung Teamviewer + Klassendesignmeeting</t>
   </si>
 </sst>
 </file>
@@ -488,7 +494,7 @@
   <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -579,7 +585,7 @@
         <v>5</v>
       </c>
       <c r="C7">
-        <f t="shared" ref="C7:C35" si="0">C6+B7</f>
+        <f t="shared" ref="C7:C21" si="0">C6+B7</f>
         <v>9.5</v>
       </c>
       <c r="D7" t="s">
@@ -827,75 +833,93 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="4">
+        <v>43849</v>
+      </c>
+      <c r="B24">
+        <v>1.5</v>
+      </c>
       <c r="C24">
         <f t="shared" ref="C24:C35" si="1">C23+B24</f>
-        <v>54.5</v>
+        <v>56</v>
+      </c>
+      <c r="D24" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="4">
+        <v>43851</v>
+      </c>
+      <c r="B25">
+        <v>6</v>
+      </c>
       <c r="C25">
         <f t="shared" si="1"/>
-        <v>54.5</v>
+        <v>62</v>
+      </c>
+      <c r="D25" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C26">
         <f t="shared" si="1"/>
-        <v>54.5</v>
+        <v>62</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C27">
         <f t="shared" si="1"/>
-        <v>54.5</v>
+        <v>62</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C28">
         <f t="shared" si="1"/>
-        <v>54.5</v>
+        <v>62</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C29">
         <f t="shared" si="1"/>
-        <v>54.5</v>
+        <v>62</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C30">
         <f t="shared" si="1"/>
-        <v>54.5</v>
+        <v>62</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C31">
         <f t="shared" si="1"/>
-        <v>54.5</v>
+        <v>62</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C32">
         <f t="shared" si="1"/>
-        <v>54.5</v>
+        <v>62</v>
       </c>
     </row>
     <row r="33" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C33">
         <f t="shared" si="1"/>
-        <v>54.5</v>
+        <v>62</v>
       </c>
     </row>
     <row r="34" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C34">
         <f t="shared" si="1"/>
-        <v>54.5</v>
+        <v>62</v>
       </c>
     </row>
     <row r="35" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C35">
         <f t="shared" si="1"/>
-        <v>54.5</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implemented decoder channel selection in UI
</commit_message>
<xml_diff>
--- a/stundenlisten/Stundenliste-AlexanderSchmid.xlsx
+++ b/stundenlisten/Stundenliste-AlexanderSchmid.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
   <si>
     <t xml:space="preserve">Studenliste von Alexander Schmid</t>
   </si>
@@ -105,6 +105,9 @@
   </si>
   <si>
     <t xml:space="preserve">Implementierung Generierung der Parameter-UI-Elemente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implementierung UI-Logik für die Decoder-Channel-Auswahl</t>
   </si>
 </sst>
 </file>
@@ -256,8 +259,8 @@
   </sheetPr>
   <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B28" activeCellId="0" sqref="B28"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -686,39 +689,48 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="8" t="n">
+        <v>44248</v>
+      </c>
+      <c r="B30" s="0" t="n">
+        <v>8</v>
+      </c>
       <c r="C30" s="0" t="n">
         <f aca="false">C29+B30</f>
-        <v>90</v>
+        <v>98</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C31" s="0" t="n">
         <f aca="false">C30+B31</f>
-        <v>90</v>
+        <v>98</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C32" s="0" t="n">
         <f aca="false">C31+B32</f>
-        <v>90</v>
+        <v>98</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C33" s="0" t="n">
         <f aca="false">C32+B33</f>
-        <v>90</v>
+        <v>98</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C34" s="0" t="n">
         <f aca="false">C33+B34</f>
-        <v>90</v>
+        <v>98</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C35" s="0" t="n">
         <f aca="false">C34+B35</f>
-        <v>90</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bugfixing and updated hours
</commit_message>
<xml_diff>
--- a/stundenlisten/Stundenliste-AlexanderSchmid.xlsx
+++ b/stundenlisten/Stundenliste-AlexanderSchmid.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
   <si>
     <t xml:space="preserve">Studenliste von Alexander Schmid</t>
   </si>
@@ -111,6 +111,9 @@
   </si>
   <si>
     <t xml:space="preserve">Debugging mit Henneke und Schneider zum Deployment der C++-Applikation auf dem RedPitaya</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Debugging mit Henneke bezüglich Senden der Decoderliste vom RedPitaya zum Client</t>
   </si>
 </sst>
 </file>
@@ -260,10 +263,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E35"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
+      <selection pane="topLeft" activeCell="D33" activeCellId="0" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -722,27 +725,78 @@
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="8" t="n">
+        <v>44252</v>
+      </c>
+      <c r="B32" s="0" t="n">
+        <v>8</v>
+      </c>
       <c r="C32" s="0" t="n">
         <f aca="false">C31+B32</f>
-        <v>106</v>
+        <v>114</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="8" t="n">
+        <v>44253</v>
+      </c>
+      <c r="B33" s="0" t="n">
+        <v>8</v>
+      </c>
       <c r="C33" s="0" t="n">
         <f aca="false">C32+B33</f>
-        <v>106</v>
+        <v>122</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="8" t="n">
+        <v>44254</v>
+      </c>
+      <c r="B34" s="0" t="n">
+        <v>8</v>
+      </c>
       <c r="C34" s="0" t="n">
         <f aca="false">C33+B34</f>
-        <v>106</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="8" t="n">
+        <v>44255</v>
+      </c>
+      <c r="B35" s="0" t="n">
+        <v>8</v>
+      </c>
       <c r="C35" s="0" t="n">
         <f aca="false">C34+B35</f>
-        <v>106</v>
+        <v>138</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="8" t="n">
+        <v>44230</v>
+      </c>
+      <c r="B36" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="C36" s="0" t="n">
+        <f aca="false">C35+B36</f>
+        <v>146</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="8" t="n">
+        <v>44231</v>
+      </c>
+      <c r="B37" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="C37" s="0" t="n">
+        <f aca="false">C36+B37</f>
+        <v>154</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added AcquirerParameters.vue to App, updated hours
</commit_message>
<xml_diff>
--- a/stundenlisten/Stundenliste-AlexanderSchmid.xlsx
+++ b/stundenlisten/Stundenliste-AlexanderSchmid.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
   <si>
     <t xml:space="preserve">Studenliste von Alexander Schmid</t>
   </si>
@@ -114,6 +114,9 @@
   </si>
   <si>
     <t xml:space="preserve">Debugging mit Henneke bezüglich Senden der Decoderliste vom RedPitaya zum Client</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recherche BeagleLogic als alternatives Board für nächste Gruppe, Implementierung UI-Logik für AcquirerParameter</t>
   </si>
 </sst>
 </file>
@@ -750,6 +753,9 @@
         <f aca="false">C32+B33</f>
         <v>122</v>
       </c>
+      <c r="D33" s="0" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="8" t="n">

</xml_diff>

<commit_message>
Updated docs and hours.
</commit_message>
<xml_diff>
--- a/stundenlisten/Stundenliste-AlexanderSchmid.xlsx
+++ b/stundenlisten/Stundenliste-AlexanderSchmid.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
   <si>
     <t xml:space="preserve">Studenliste von Alexander Schmid</t>
   </si>
@@ -274,8 +274,8 @@
   </sheetPr>
   <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D36" activeCellId="0" sqref="D36"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D37" activeCellId="0" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -795,14 +795,17 @@
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="8" t="n">
-        <v>44230</v>
+        <v>44256</v>
       </c>
       <c r="B36" s="0" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C36" s="0" t="n">
         <f aca="false">C35+B36</f>
-        <v>146</v>
+        <v>141</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -814,7 +817,7 @@
       </c>
       <c r="C37" s="0" t="n">
         <f aca="false">C36+B37</f>
-        <v>154</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reencoded video, built Abgabe.zip, rebuild Documentation.pdf
</commit_message>
<xml_diff>
--- a/stundenlisten/Stundenliste-AlexanderSchmid.xlsx
+++ b/stundenlisten/Stundenliste-AlexanderSchmid.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="36">
   <si>
     <t xml:space="preserve">Studenliste von Alexander Schmid</t>
   </si>
@@ -126,6 +126,9 @@
   </si>
   <si>
     <t xml:space="preserve">Aufnahme Video, Verwaltung der Dateien für die Abgabe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Videoschnitt mit Sebastian</t>
   </si>
 </sst>
 </file>
@@ -275,10 +278,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D38" activeCellId="0" sqref="D38"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D39" activeCellId="0" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -824,6 +827,21 @@
       </c>
       <c r="D37" s="0" t="s">
         <v>34</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="8" t="n">
+        <v>44258</v>
+      </c>
+      <c r="B38" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C38" s="0" t="n">
+        <f aca="false">C37+B38</f>
+        <v>150</v>
+      </c>
+      <c r="D38" s="0" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed conflict between jquery and jquery ui.
</commit_message>
<xml_diff>
--- a/stundenlisten/Stundenliste-AlexanderSchmid.xlsx
+++ b/stundenlisten/Stundenliste-AlexanderSchmid.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t xml:space="preserve">Studenliste von Alexander Schmid</t>
   </si>
@@ -71,6 +71,9 @@
   </si>
   <si>
     <t xml:space="preserve">Formattierung der Sampleraten mit Einheiten via mathjs hinzugefügt.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Debugging eines Konflikts zwischen jQuery und jQueryUI</t>
   </si>
 </sst>
 </file>
@@ -227,10 +230,10 @@
   <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
+      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.56640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.85"/>
@@ -402,11 +405,17 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="n">
-        <v>44159</v>
+        <v>44337</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>5</v>
       </c>
       <c r="C13" s="0" t="n">
         <f aca="false">C12+B13</f>
-        <v>34</v>
+        <v>39</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -415,7 +424,7 @@
       </c>
       <c r="C14" s="0" t="n">
         <f aca="false">C13+B14</f>
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -424,7 +433,7 @@
       </c>
       <c r="C15" s="0" t="n">
         <f aca="false">C14+B15</f>
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -433,7 +442,7 @@
       </c>
       <c r="C16" s="0" t="n">
         <f aca="false">C15+B16</f>
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -442,7 +451,7 @@
       </c>
       <c r="C17" s="0" t="n">
         <f aca="false">C16+B17</f>
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -451,7 +460,7 @@
       </c>
       <c r="C18" s="0" t="n">
         <f aca="false">C17+B18</f>
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -460,7 +469,7 @@
       </c>
       <c r="C19" s="0" t="n">
         <f aca="false">C18+B19</f>
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -469,7 +478,7 @@
       </c>
       <c r="C20" s="0" t="n">
         <f aca="false">C19+B20</f>
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -478,7 +487,7 @@
       </c>
       <c r="C21" s="0" t="n">
         <f aca="false">C20+B21</f>
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -487,7 +496,7 @@
       </c>
       <c r="C22" s="0" t="n">
         <f aca="false">C20+B22</f>
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -496,7 +505,7 @@
       </c>
       <c r="C23" s="0" t="n">
         <f aca="false">C22+B23</f>
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -505,7 +514,7 @@
       </c>
       <c r="C24" s="0" t="n">
         <f aca="false">C23+B24</f>
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -514,7 +523,7 @@
       </c>
       <c r="C25" s="0" t="n">
         <f aca="false">C24+B25</f>
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -523,7 +532,7 @@
       </c>
       <c r="C26" s="0" t="n">
         <f aca="false">C25+B26</f>
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -532,7 +541,7 @@
       </c>
       <c r="C27" s="0" t="n">
         <f aca="false">C26+B27</f>
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -541,7 +550,7 @@
       </c>
       <c r="C28" s="0" t="n">
         <f aca="false">C27+B28</f>
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -550,7 +559,7 @@
       </c>
       <c r="C29" s="0" t="n">
         <f aca="false">C28+B29</f>
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -559,7 +568,7 @@
       </c>
       <c r="C30" s="0" t="n">
         <f aca="false">C29+B30</f>
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -568,7 +577,7 @@
       </c>
       <c r="C31" s="0" t="n">
         <f aca="false">C30+B31</f>
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -577,7 +586,7 @@
       </c>
       <c r="C32" s="0" t="n">
         <f aca="false">C31+B32</f>
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -586,7 +595,7 @@
       </c>
       <c r="C33" s="0" t="n">
         <f aca="false">C32+B33</f>
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -595,7 +604,7 @@
       </c>
       <c r="C34" s="0" t="n">
         <f aca="false">C33+B34</f>
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -604,7 +613,7 @@
       </c>
       <c r="C35" s="0" t="n">
         <f aca="false">C34+B35</f>
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -613,7 +622,7 @@
       </c>
       <c r="C36" s="0" t="n">
         <f aca="false">C35+B36</f>
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -622,7 +631,7 @@
       </c>
       <c r="C37" s="0" t="n">
         <f aca="false">C36+B37</f>
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -631,7 +640,7 @@
       </c>
       <c r="C38" s="0" t="n">
         <f aca="false">C37+B38</f>
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -641,7 +650,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
Updated AcquirerParameters and hours.
</commit_message>
<xml_diff>
--- a/stundenlisten/Stundenliste-AlexanderSchmid.xlsx
+++ b/stundenlisten/Stundenliste-AlexanderSchmid.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t xml:space="preserve">Studenliste von Alexander Schmid</t>
   </si>
@@ -77,6 +77,15 @@
   </si>
   <si>
     <t xml:space="preserve">SRDChosenOptions Signal zu einem Parameter refactored</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Internes Meeting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Debugging des HTTP-Servers im RedpitayaStub (Resultat: HTTP-Server wurde entfernt, nur WebSocket bleibt=</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implementierung AcquirerOptions: Einheitenlogik ist vollständig, Inputvalidierung noch zu tun</t>
   </si>
 </sst>
 </file>
@@ -233,10 +242,10 @@
   <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
+      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.55859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.85"/>
@@ -423,7 +432,7 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="n">
-        <v>43979</v>
+        <v>44344</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>2</v>
@@ -438,29 +447,47 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="n">
-        <v>44165</v>
+        <v>44351</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="C15" s="0" t="n">
         <f aca="false">C14+B15</f>
-        <v>41</v>
+        <v>42</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="n">
-        <v>44168</v>
+        <v>44351</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>2</v>
       </c>
       <c r="C16" s="0" t="n">
         <f aca="false">C15+B16</f>
-        <v>41</v>
+        <v>44</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="n">
-        <v>44173</v>
+        <v>44353</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>6</v>
       </c>
       <c r="C17" s="0" t="n">
         <f aca="false">C16+B17</f>
-        <v>41</v>
+        <v>50</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -469,7 +496,7 @@
       </c>
       <c r="C18" s="0" t="n">
         <f aca="false">C17+B18</f>
-        <v>41</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -478,7 +505,7 @@
       </c>
       <c r="C19" s="0" t="n">
         <f aca="false">C18+B19</f>
-        <v>41</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -487,7 +514,7 @@
       </c>
       <c r="C20" s="0" t="n">
         <f aca="false">C19+B20</f>
-        <v>41</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -496,7 +523,7 @@
       </c>
       <c r="C21" s="0" t="n">
         <f aca="false">C20+B21</f>
-        <v>41</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -505,7 +532,7 @@
       </c>
       <c r="C22" s="0" t="n">
         <f aca="false">C20+B22</f>
-        <v>41</v>
+        <v>50</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -514,7 +541,7 @@
       </c>
       <c r="C23" s="0" t="n">
         <f aca="false">C22+B23</f>
-        <v>41</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -523,7 +550,7 @@
       </c>
       <c r="C24" s="0" t="n">
         <f aca="false">C23+B24</f>
-        <v>41</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -532,7 +559,7 @@
       </c>
       <c r="C25" s="0" t="n">
         <f aca="false">C24+B25</f>
-        <v>41</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -541,7 +568,7 @@
       </c>
       <c r="C26" s="0" t="n">
         <f aca="false">C25+B26</f>
-        <v>41</v>
+        <v>50</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -550,7 +577,7 @@
       </c>
       <c r="C27" s="0" t="n">
         <f aca="false">C26+B27</f>
-        <v>41</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -559,7 +586,7 @@
       </c>
       <c r="C28" s="0" t="n">
         <f aca="false">C27+B28</f>
-        <v>41</v>
+        <v>50</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -568,7 +595,7 @@
       </c>
       <c r="C29" s="0" t="n">
         <f aca="false">C28+B29</f>
-        <v>41</v>
+        <v>50</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -577,7 +604,7 @@
       </c>
       <c r="C30" s="0" t="n">
         <f aca="false">C29+B30</f>
-        <v>41</v>
+        <v>50</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -586,7 +613,7 @@
       </c>
       <c r="C31" s="0" t="n">
         <f aca="false">C30+B31</f>
-        <v>41</v>
+        <v>50</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -595,7 +622,7 @@
       </c>
       <c r="C32" s="0" t="n">
         <f aca="false">C31+B32</f>
-        <v>41</v>
+        <v>50</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -604,7 +631,7 @@
       </c>
       <c r="C33" s="0" t="n">
         <f aca="false">C32+B33</f>
-        <v>41</v>
+        <v>50</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -613,7 +640,7 @@
       </c>
       <c r="C34" s="0" t="n">
         <f aca="false">C33+B34</f>
-        <v>41</v>
+        <v>50</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -622,7 +649,7 @@
       </c>
       <c r="C35" s="0" t="n">
         <f aca="false">C34+B35</f>
-        <v>41</v>
+        <v>50</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -631,7 +658,7 @@
       </c>
       <c r="C36" s="0" t="n">
         <f aca="false">C35+B36</f>
-        <v>41</v>
+        <v>50</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -640,7 +667,7 @@
       </c>
       <c r="C37" s="0" t="n">
         <f aca="false">C36+B37</f>
-        <v>41</v>
+        <v>50</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -649,7 +676,7 @@
       </c>
       <c r="C38" s="0" t="n">
         <f aca="false">C37+B38</f>
-        <v>41</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implemented input validation for acquirer parameters
</commit_message>
<xml_diff>
--- a/stundenlisten/Stundenliste-AlexanderSchmid.xlsx
+++ b/stundenlisten/Stundenliste-AlexanderSchmid.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t xml:space="preserve">Studenliste von Alexander Schmid</t>
   </si>
@@ -86,6 +86,9 @@
   </si>
   <si>
     <t xml:space="preserve">Implementierung AcquirerOptions: Einheitenlogik ist vollständig, Inputvalidierung noch zu tun</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implementierung der Inputvalidierung der AcquirerOptions</t>
   </si>
 </sst>
 </file>
@@ -242,10 +245,10 @@
   <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
+      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.85"/>
@@ -492,11 +495,17 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="6" t="n">
-        <v>44177</v>
+        <v>44357</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>3</v>
       </c>
       <c r="C18" s="0" t="n">
         <f aca="false">C17+B18</f>
-        <v>50</v>
+        <v>53</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -505,7 +514,7 @@
       </c>
       <c r="C19" s="0" t="n">
         <f aca="false">C18+B19</f>
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -514,7 +523,7 @@
       </c>
       <c r="C20" s="0" t="n">
         <f aca="false">C19+B20</f>
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -523,7 +532,7 @@
       </c>
       <c r="C21" s="0" t="n">
         <f aca="false">C20+B21</f>
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -532,7 +541,7 @@
       </c>
       <c r="C22" s="0" t="n">
         <f aca="false">C20+B22</f>
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -541,7 +550,7 @@
       </c>
       <c r="C23" s="0" t="n">
         <f aca="false">C22+B23</f>
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -550,7 +559,7 @@
       </c>
       <c r="C24" s="0" t="n">
         <f aca="false">C23+B24</f>
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -559,7 +568,7 @@
       </c>
       <c r="C25" s="0" t="n">
         <f aca="false">C24+B25</f>
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -568,7 +577,7 @@
       </c>
       <c r="C26" s="0" t="n">
         <f aca="false">C25+B26</f>
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -577,7 +586,7 @@
       </c>
       <c r="C27" s="0" t="n">
         <f aca="false">C26+B27</f>
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -586,7 +595,7 @@
       </c>
       <c r="C28" s="0" t="n">
         <f aca="false">C27+B28</f>
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -595,7 +604,7 @@
       </c>
       <c r="C29" s="0" t="n">
         <f aca="false">C28+B29</f>
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -604,7 +613,7 @@
       </c>
       <c r="C30" s="0" t="n">
         <f aca="false">C29+B30</f>
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -613,7 +622,7 @@
       </c>
       <c r="C31" s="0" t="n">
         <f aca="false">C30+B31</f>
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -622,7 +631,7 @@
       </c>
       <c r="C32" s="0" t="n">
         <f aca="false">C31+B32</f>
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -631,7 +640,7 @@
       </c>
       <c r="C33" s="0" t="n">
         <f aca="false">C32+B33</f>
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -640,7 +649,7 @@
       </c>
       <c r="C34" s="0" t="n">
         <f aca="false">C33+B34</f>
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -649,7 +658,7 @@
       </c>
       <c r="C35" s="0" t="n">
         <f aca="false">C34+B35</f>
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -658,7 +667,7 @@
       </c>
       <c r="C36" s="0" t="n">
         <f aca="false">C35+B36</f>
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -667,7 +676,7 @@
       </c>
       <c r="C37" s="0" t="n">
         <f aca="false">C36+B37</f>
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -676,7 +685,7 @@
       </c>
       <c r="C38" s="0" t="n">
         <f aca="false">C37+B38</f>
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added sending of channelMap
</commit_message>
<xml_diff>
--- a/stundenlisten/Stundenliste-AlexanderSchmid.xlsx
+++ b/stundenlisten/Stundenliste-AlexanderSchmid.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t xml:space="preserve">Studenliste von Alexander Schmid</t>
   </si>
@@ -89,6 +89,9 @@
   </si>
   <si>
     <t xml:space="preserve">Implementierung der Inputvalidierung der AcquirerOptions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implementierung vom Senden der ChannelMap an den RedPitaya</t>
   </si>
 </sst>
 </file>
@@ -245,10 +248,10 @@
   <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
+      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.85"/>
@@ -510,11 +513,17 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="6" t="n">
-        <v>44182</v>
+        <v>44373</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>4</v>
       </c>
       <c r="C19" s="0" t="n">
         <f aca="false">C18+B19</f>
-        <v>53</v>
+        <v>57</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -523,7 +532,7 @@
       </c>
       <c r="C20" s="0" t="n">
         <f aca="false">C19+B20</f>
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -532,7 +541,7 @@
       </c>
       <c r="C21" s="0" t="n">
         <f aca="false">C20+B21</f>
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -541,7 +550,7 @@
       </c>
       <c r="C22" s="0" t="n">
         <f aca="false">C20+B22</f>
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -550,7 +559,7 @@
       </c>
       <c r="C23" s="0" t="n">
         <f aca="false">C22+B23</f>
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -559,7 +568,7 @@
       </c>
       <c r="C24" s="0" t="n">
         <f aca="false">C23+B24</f>
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -568,7 +577,7 @@
       </c>
       <c r="C25" s="0" t="n">
         <f aca="false">C24+B25</f>
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -577,7 +586,7 @@
       </c>
       <c r="C26" s="0" t="n">
         <f aca="false">C25+B26</f>
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -586,7 +595,7 @@
       </c>
       <c r="C27" s="0" t="n">
         <f aca="false">C26+B27</f>
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -595,7 +604,7 @@
       </c>
       <c r="C28" s="0" t="n">
         <f aca="false">C27+B28</f>
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -604,7 +613,7 @@
       </c>
       <c r="C29" s="0" t="n">
         <f aca="false">C28+B29</f>
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -613,7 +622,7 @@
       </c>
       <c r="C30" s="0" t="n">
         <f aca="false">C29+B30</f>
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -622,7 +631,7 @@
       </c>
       <c r="C31" s="0" t="n">
         <f aca="false">C30+B31</f>
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -631,7 +640,7 @@
       </c>
       <c r="C32" s="0" t="n">
         <f aca="false">C31+B32</f>
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -640,7 +649,7 @@
       </c>
       <c r="C33" s="0" t="n">
         <f aca="false">C32+B33</f>
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -649,7 +658,7 @@
       </c>
       <c r="C34" s="0" t="n">
         <f aca="false">C33+B34</f>
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -658,7 +667,7 @@
       </c>
       <c r="C35" s="0" t="n">
         <f aca="false">C34+B35</f>
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -667,7 +676,7 @@
       </c>
       <c r="C36" s="0" t="n">
         <f aca="false">C35+B36</f>
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -676,7 +685,7 @@
       </c>
       <c r="C37" s="0" t="n">
         <f aca="false">C36+B37</f>
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -685,7 +694,7 @@
       </c>
       <c r="C38" s="0" t="n">
         <f aca="false">C37+B38</f>
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finalized display of measured data
</commit_message>
<xml_diff>
--- a/stundenlisten/Stundenliste-AlexanderSchmid.xlsx
+++ b/stundenlisten/Stundenliste-AlexanderSchmid.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t xml:space="preserve">Studenliste von Alexander Schmid</t>
   </si>
@@ -107,6 +107,12 @@
   </si>
   <si>
     <t xml:space="preserve">Fertigstellen des Progress Spinners im Start-Analyzing Button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implementierung des sendens von Beispieldaten des MeasuredData-Signals im RepitayaStub</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implementierung des Empfangens der MeasuredData in der UI und Anzeige via der uPlot-Chart</t>
   </si>
 </sst>
 </file>
@@ -263,10 +269,10 @@
   <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D25" activeCellId="0" sqref="D25"/>
+      <selection pane="topLeft" activeCell="D28" activeCellId="0" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.85"/>
@@ -633,20 +639,32 @@
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="6" t="n">
-        <v>44224</v>
+        <v>44429</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <v>8</v>
       </c>
       <c r="C26" s="0" t="n">
         <f aca="false">C25+B26</f>
-        <v>86</v>
+        <v>94</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="9" t="n">
-        <v>44244</v>
+        <v>44430</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <v>8</v>
       </c>
       <c r="C27" s="0" t="n">
         <f aca="false">C26+B27</f>
-        <v>86</v>
+        <v>102</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -655,7 +673,7 @@
       </c>
       <c r="C28" s="0" t="n">
         <f aca="false">C27+B28</f>
-        <v>86</v>
+        <v>102</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -664,7 +682,7 @@
       </c>
       <c r="C29" s="0" t="n">
         <f aca="false">C28+B29</f>
-        <v>86</v>
+        <v>102</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -673,7 +691,7 @@
       </c>
       <c r="C30" s="0" t="n">
         <f aca="false">C29+B30</f>
-        <v>86</v>
+        <v>102</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -682,7 +700,7 @@
       </c>
       <c r="C31" s="0" t="n">
         <f aca="false">C30+B31</f>
-        <v>86</v>
+        <v>102</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -691,7 +709,7 @@
       </c>
       <c r="C32" s="0" t="n">
         <f aca="false">C31+B32</f>
-        <v>86</v>
+        <v>102</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -700,7 +718,7 @@
       </c>
       <c r="C33" s="0" t="n">
         <f aca="false">C32+B33</f>
-        <v>86</v>
+        <v>102</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -709,7 +727,7 @@
       </c>
       <c r="C34" s="0" t="n">
         <f aca="false">C33+B34</f>
-        <v>86</v>
+        <v>102</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -718,7 +736,7 @@
       </c>
       <c r="C35" s="0" t="n">
         <f aca="false">C34+B35</f>
-        <v>86</v>
+        <v>102</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -727,7 +745,7 @@
       </c>
       <c r="C36" s="0" t="n">
         <f aca="false">C35+B36</f>
-        <v>86</v>
+        <v>102</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -736,7 +754,7 @@
       </c>
       <c r="C37" s="0" t="n">
         <f aca="false">C36+B37</f>
-        <v>86</v>
+        <v>102</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -745,7 +763,7 @@
       </c>
       <c r="C38" s="0" t="n">
         <f aca="false">C37+B38</f>
-        <v>86</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Potentially fixed error of channels not appearing before measuredData is received
</commit_message>
<xml_diff>
--- a/stundenlisten/Stundenliste-AlexanderSchmid.xlsx
+++ b/stundenlisten/Stundenliste-AlexanderSchmid.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t xml:space="preserve">Studenliste von Alexander Schmid</t>
   </si>
@@ -113,6 +113,12 @@
   </si>
   <si>
     <t xml:space="preserve">Implementierung des Empfangens der MeasuredData in der UI und Anzeige via der uPlot-Chart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weitere Implementierung der Anzeige der MeasuredData</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bugfixing der Anzeige der MeasuredData</t>
   </si>
 </sst>
 </file>
@@ -121,9 +127,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
+    <numFmt numFmtId="165" formatCode="D/M/YYYY"/>
     <numFmt numFmtId="166" formatCode="0.00"/>
-    <numFmt numFmtId="167" formatCode="mm/dd/yy"/>
+    <numFmt numFmtId="167" formatCode="DD/MM/YY"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -251,33 +257,34 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D28" activeCellId="0" sqref="D28"/>
+      <selection pane="topLeft" activeCell="D29" activeCellId="0" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="56.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="10.5"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -669,20 +676,32 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="9" t="n">
-        <v>44245</v>
+        <v>44443</v>
+      </c>
+      <c r="B28" s="0" t="n">
+        <v>8</v>
       </c>
       <c r="C28" s="0" t="n">
         <f aca="false">C27+B28</f>
-        <v>102</v>
+        <v>110</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="9" t="n">
-        <v>44247</v>
+        <v>44444</v>
+      </c>
+      <c r="B29" s="0" t="n">
+        <v>8</v>
       </c>
       <c r="C29" s="0" t="n">
         <f aca="false">C28+B29</f>
-        <v>102</v>
+        <v>118</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -691,7 +710,7 @@
       </c>
       <c r="C30" s="0" t="n">
         <f aca="false">C29+B30</f>
-        <v>102</v>
+        <v>118</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -700,7 +719,7 @@
       </c>
       <c r="C31" s="0" t="n">
         <f aca="false">C30+B31</f>
-        <v>102</v>
+        <v>118</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -709,7 +728,7 @@
       </c>
       <c r="C32" s="0" t="n">
         <f aca="false">C31+B32</f>
-        <v>102</v>
+        <v>118</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -718,7 +737,7 @@
       </c>
       <c r="C33" s="0" t="n">
         <f aca="false">C32+B33</f>
-        <v>102</v>
+        <v>118</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -727,7 +746,7 @@
       </c>
       <c r="C34" s="0" t="n">
         <f aca="false">C33+B34</f>
-        <v>102</v>
+        <v>118</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -736,7 +755,7 @@
       </c>
       <c r="C35" s="0" t="n">
         <f aca="false">C34+B35</f>
-        <v>102</v>
+        <v>118</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -745,7 +764,7 @@
       </c>
       <c r="C36" s="0" t="n">
         <f aca="false">C35+B36</f>
-        <v>102</v>
+        <v>118</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -754,7 +773,7 @@
       </c>
       <c r="C37" s="0" t="n">
         <f aca="false">C36+B37</f>
-        <v>102</v>
+        <v>118</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -763,7 +782,7 @@
       </c>
       <c r="C38" s="0" t="n">
         <f aca="false">C37+B38</f>
-        <v>102</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -773,7 +792,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>